<commit_message>
updates for 2019... not quite finished though, need to see how round 1 plays out
</commit_message>
<xml_diff>
--- a/ImportCSV/2019/Round1-Snapper.xlsx
+++ b/ImportCSV/2019/Round1-Snapper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WSLapp\ImportCSV\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calhamd\Documents\WSL_Fantasy\ImportCSV\2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50E64D4F-B23A-492A-A3DE-9B20EB802AB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EDB4B6-3F9A-47BA-AEBC-C20B352EBE31}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-6210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2152" yWindow="2723" windowWidth="8865" windowHeight="8325" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Round1-Snapper" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Round1-Snapper'!$A$1:$G$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$A$1:$D$38</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="65">
   <si>
     <t>Odds</t>
   </si>
@@ -208,12 +209,27 @@
   <si>
     <t>Aus</t>
   </si>
+  <si>
+    <t>Ath</t>
+  </si>
+  <si>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Reef Heazlewood</t>
+  </si>
+  <si>
+    <t>Mateus Herdy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,14 +369,6 @@
       <color rgb="FF404040"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -681,7 +689,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -724,9 +732,8 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -734,17 +741,14 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -778,7 +782,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -7652,6 +7655,125 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="190500"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9525" cy="9525"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://mct.fantasy.worldsurfleague.com/cache/img/placeholder-1x1_1488162224.gif">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tgtFrame="_blank"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD2625B5-3EA3-46DB-A9EF-CD1DF1E0384D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2200275" y="6619875"/>
+          <a:ext cx="9525" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9525" cy="9525"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="http://mct.fantasy.worldsurfleague.com/cache/img/placeholder-1x1_1488162224.gif">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tgtFrame="_blank"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47578799-34CD-4867-BE0A-D1141CADCEAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2200275" y="6619875"/>
           <a:ext cx="9525" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7973,19 +8095,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G37" sqref="G2:G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" customWidth="1"/>
     <col min="4" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8008,7 +8130,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C2,Odds!B:B),201)</f>
         <v>5</v>
@@ -8035,7 +8157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C3,Odds!B:B),201)</f>
         <v>6</v>
@@ -8062,7 +8184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A4">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C4,Odds!B:B),201)</f>
         <v>6.5</v>
@@ -8083,7 +8205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C5,Odds!B:B),201)</f>
         <v>7</v>
@@ -8110,7 +8232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C6,Odds!B:B),201)</f>
         <v>9</v>
@@ -8137,7 +8259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C7,Odds!B:B),201)</f>
         <v>15</v>
@@ -8164,7 +8286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C8,Odds!B:B),201)</f>
         <v>21</v>
@@ -8191,7 +8313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C9,Odds!B:B),201)</f>
         <v>21</v>
@@ -8218,7 +8340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C10,Odds!B:B),201)</f>
         <v>26</v>
@@ -8245,7 +8367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A11">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C11,Odds!B:B),201)</f>
         <v>26</v>
@@ -8266,7 +8388,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C12,Odds!B:B),201)</f>
         <v>34</v>
@@ -8293,7 +8415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C13,Odds!B:B),201)</f>
         <v>34</v>
@@ -8320,7 +8442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C14,Odds!B:B),201)</f>
         <v>34</v>
@@ -8347,7 +8469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A15">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C15,Odds!B:B),201)</f>
         <v>36</v>
@@ -8368,7 +8490,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C16,Odds!B:B),201)</f>
         <v>41</v>
@@ -8395,7 +8517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A17">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C17,Odds!B:B),201)</f>
         <v>41</v>
@@ -8419,7 +8541,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C18,Odds!B:B),201)</f>
         <v>51</v>
@@ -8446,7 +8568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C19,Odds!B:B),201)</f>
         <v>51</v>
@@ -8473,7 +8595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C20,Odds!B:B),201)</f>
         <v>61</v>
@@ -8500,7 +8622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C21,Odds!B:B),201)</f>
         <v>61</v>
@@ -8527,7 +8649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C22,Odds!B:B),201)</f>
         <v>61</v>
@@ -8554,7 +8676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C23,Odds!B:B),201)</f>
         <v>67</v>
@@ -8581,7 +8703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A24">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C24,Odds!B:B),201)</f>
         <v>76</v>
@@ -8602,7 +8724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A25">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C25,Odds!B:B),201)</f>
         <v>81</v>
@@ -8623,7 +8745,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C26,Odds!B:B),201)</f>
         <v>101</v>
@@ -8650,7 +8772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C27,Odds!B:B),201)</f>
         <v>101</v>
@@ -8677,7 +8799,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A28">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C28,Odds!B:B),201)</f>
         <v>101</v>
@@ -8698,7 +8820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A29">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C29,Odds!B:B),201)</f>
         <v>101</v>
@@ -8719,7 +8841,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A30">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C30,Odds!B:B),201)</f>
         <v>101</v>
@@ -8740,7 +8862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A31">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C31,Odds!B:B),201)</f>
         <v>101</v>
@@ -8761,7 +8883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C32,Odds!B:B),201)</f>
         <v>201</v>
@@ -8788,7 +8910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C33,Odds!B:B),201)</f>
         <v>201</v>
@@ -8815,7 +8937,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C34,Odds!B:B),201)</f>
         <v>201</v>
@@ -8836,7 +8958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C35,Odds!B:B),201)</f>
         <v>201</v>
@@ -8857,7 +8979,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A36">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C36,Odds!B:B),201)</f>
         <v>176</v>
@@ -8878,7 +9000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.45">
       <c r="A37">
         <f>IFERROR(AVERAGEIF(Odds!A:A,C37,Odds!B:B),201)</f>
         <v>201</v>
@@ -8899,7 +9021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E38" t="str">
         <f>IFERROR(INDEX(Tier!B:B,MATCH('Round1-Snapper'!C38,Tier!A:A,0)),"")</f>
         <v/>
@@ -8930,277 +9052,277 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="2" width="22.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B1">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B3">
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B8">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B9">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B10">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B11">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:2" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B12">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B13">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B14">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B16">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B17">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B18">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B19">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B20">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B21">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B22">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B23">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B24">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B25">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B26">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B27">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B28">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B29">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B30">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B31">
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B32">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:2" ht="15.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A33" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B33">
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B34">
@@ -9221,13 +9343,13 @@
       <selection activeCell="A37" sqref="A2:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.3984375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
@@ -9235,7 +9357,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -9243,7 +9365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -9251,7 +9373,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -9259,7 +9381,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -9267,7 +9389,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -9275,7 +9397,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -9283,7 +9405,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -9291,7 +9413,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -9299,7 +9421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -9307,7 +9429,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -9315,7 +9437,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
@@ -9323,7 +9445,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -9331,7 +9453,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -9339,7 +9461,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -9347,7 +9469,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>48</v>
       </c>
@@ -9355,7 +9477,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -9363,7 +9485,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -9371,7 +9493,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -9379,7 +9501,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -9387,7 +9509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -9395,7 +9517,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
@@ -9403,7 +9525,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -9411,7 +9533,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -9419,7 +9541,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -9427,7 +9549,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -9435,7 +9557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -9443,7 +9565,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
@@ -9451,7 +9573,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
@@ -9459,7 +9581,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
@@ -9467,7 +9589,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -9475,7 +9597,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -9483,7 +9605,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -9491,7 +9613,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -9499,7 +9621,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>55</v>
       </c>
@@ -9507,7 +9629,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
@@ -9515,114 +9637,114 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="84" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="87" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="90" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="91" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="92" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="94" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="96" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="97" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="98" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="99" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="101" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="102" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="103" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="104" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="105" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="106" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="107" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="108" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="109" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="110" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="111" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="112" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="114" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="115" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="116" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="117" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="118" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="119" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="120" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="121" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="122" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="123" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="124" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="125" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="126" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="127" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="128" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="129" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="130" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="131" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="132" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="133" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="134" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="135" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="136" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="137" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="138" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="139" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="140" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="141" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="142" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="143" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="144" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="145" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <sortState ref="A1:B1047842">
     <sortCondition ref="B1:B1047842"/>
@@ -9637,17 +9759,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AEC66BE-4756-4779-8F6D-E036832303F8}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>42</v>
       </c>
@@ -9655,7 +9777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -9666,7 +9788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -9677,7 +9799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -9688,7 +9810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -9699,7 +9821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -9710,7 +9832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -9721,7 +9843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -9732,7 +9854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -9743,7 +9865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -9754,7 +9876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -9765,7 +9887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -9776,7 +9898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -9787,7 +9909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -9798,7 +9920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -9809,7 +9931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -9820,7 +9942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -9831,7 +9953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -9842,7 +9964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -9853,7 +9975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -9864,12 +9986,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -9880,7 +10002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -9891,7 +10013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -9902,7 +10024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -9913,7 +10035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -9924,7 +10046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -9935,7 +10057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -9946,7 +10068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -9957,7 +10079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -9968,7 +10090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -9979,7 +10101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -9990,7 +10112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -10001,7 +10123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -10012,7 +10134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -10023,7 +10145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -10034,7 +10156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -10045,7 +10167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>56</v>
       </c>
@@ -10056,83 +10178,83 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B44">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B46">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1"/>
       <c r="C52">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C53">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C54">
         <v>6</v>
       </c>
@@ -10144,224 +10266,475 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E30CDFE-8C38-4384-AE43-3945DDEA4A24}">
-  <dimension ref="A1:A34"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D3:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="http://www.worldsurfleague.com/athletes/1085/gabriel-medina" xr:uid="{874D468E-C67E-4747-B630-2C9CB7194685}"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://www.worldsurfleague.com/athletes/763/julian-wilson" xr:uid="{572452F8-CBF2-4F41-9250-5A4FAE399614}"/>
-    <hyperlink ref="A3" r:id="rId3" display="http://www.worldsurfleague.com/athletes/1456/filipe-toledo" xr:uid="{E0C61DD2-1022-4C3C-8552-5EA5869E53EA}"/>
-    <hyperlink ref="A4" r:id="rId4" display="http://www.worldsurfleague.com/athletes/1737/italo-ferreira" xr:uid="{A0AE1052-705A-4C72-B5C7-5BF42535E8B6}"/>
-    <hyperlink ref="A5" r:id="rId5" display="http://www.worldsurfleague.com/athletes/564/jordy-smith" xr:uid="{BF200B25-62A9-45C3-B39F-20E89C6EAADB}"/>
-    <hyperlink ref="A6" r:id="rId6" display="http://www.worldsurfleague.com/athletes/297/owen-wright" xr:uid="{84C18449-5790-4F31-BE92-427227A92128}"/>
-    <hyperlink ref="A7" r:id="rId7" display="http://www.worldsurfleague.com/athletes/1215/conner-coffin" xr:uid="{13BC4C36-19BE-425D-9DF2-6C32EBADEA71}"/>
-    <hyperlink ref="A8" r:id="rId8" display="http://www.worldsurfleague.com/athletes/593/michel-bourez" xr:uid="{21E8EBF3-85F6-4ED5-A3F5-F58FCED513F9}"/>
-    <hyperlink ref="A9" r:id="rId9" display="http://www.worldsurfleague.com/athletes/2817/wade-carmichael" xr:uid="{7C515A9C-F39C-457B-91F5-A0A8030FFA14}"/>
-    <hyperlink ref="A10" r:id="rId10" display="http://www.worldsurfleague.com/athletes/3896/kanoa-igarashi" xr:uid="{B1CD2709-65AF-4143-84EE-E81A3751C8B8}"/>
-    <hyperlink ref="A11" r:id="rId11" display="http://www.worldsurfleague.com/athletes/1164/kolohe-andino" xr:uid="{436FD821-DCE4-4C84-8A03-8616F7777E53}"/>
-    <hyperlink ref="A12" r:id="rId12" display="http://www.worldsurfleague.com/athletes/3830/mikey-wright" xr:uid="{DCD1B884-F18F-4588-9653-F196B15FBF42}"/>
-    <hyperlink ref="A13" r:id="rId13" display="http://www.worldsurfleague.com/athletes/199/john-john-florence" xr:uid="{3A61C47C-38C1-42EE-97E4-140C35E44A5C}"/>
-    <hyperlink ref="A14" r:id="rId14" display="http://www.worldsurfleague.com/athletes/622/willian-cardoso" xr:uid="{CAA1F142-9979-48FD-B499-5D07B8E3F5BC}"/>
-    <hyperlink ref="A15" r:id="rId15" display="http://www.worldsurfleague.com/athletes/14/sebastian-zietz" xr:uid="{9E689268-9A5C-408E-A9C5-0D9F3DDA10DD}"/>
-    <hyperlink ref="A16" r:id="rId16" display="http://www.worldsurfleague.com/athletes/2251/michael-rodrigues" xr:uid="{BDB79456-7058-4BC7-962B-ED901DFDFD53}"/>
-    <hyperlink ref="A17" r:id="rId17" display="http://www.worldsurfleague.com/athletes/562/jeremy-flores" xr:uid="{0E02C189-0242-4DDD-B1D1-492D4ACE3C55}"/>
-    <hyperlink ref="A18" r:id="rId18" display="http://www.worldsurfleague.com/athletes/575/adrian-buchan" xr:uid="{FB0673E8-972D-4297-84BD-7DCE41CA138C}"/>
-    <hyperlink ref="A19" r:id="rId19" display="http://www.worldsurfleague.com/athletes/3165/griffin-colapinto" xr:uid="{E9AEBC93-4EA8-4CDC-9EBC-FED1D9283D74}"/>
-    <hyperlink ref="A20" r:id="rId20" display="http://www.worldsurfleague.com/athletes/13/adriano-de-souza" xr:uid="{4B0A8182-A990-4F48-A275-656FD08747E0}"/>
-    <hyperlink ref="A21" r:id="rId21" display="http://www.worldsurfleague.com/athletes/1957/ezekiel-lau" xr:uid="{95D1D5E5-8780-4A24-9A61-E0E140155939}"/>
-    <hyperlink ref="A22" r:id="rId22" display="http://www.worldsurfleague.com/athletes/3994/yago-dora" xr:uid="{7B94095F-5FC5-4620-A361-EAA4ECEAC8D7}"/>
-    <hyperlink ref="A23" r:id="rId23" display="http://www.worldsurfleague.com/athletes/621/joan-duru" xr:uid="{B9E7AF40-FEDD-4CB1-AAFD-14007216D38C}"/>
-    <hyperlink ref="A24" r:id="rId24" display="http://www.worldsurfleague.com/athletes/3955/seth-moniz" xr:uid="{D2552A7F-7302-4990-B049-8F3DC68FF888}"/>
-    <hyperlink ref="A25" r:id="rId25" display="http://www.worldsurfleague.com/athletes/1760/ryan-callinan" xr:uid="{67DC178F-3F0F-4734-92DD-CE332EBCD062}"/>
-    <hyperlink ref="A26" r:id="rId26" display="http://www.worldsurfleague.com/athletes/482/peterson-crisanto" xr:uid="{8138641F-F168-421B-8002-C83E879B4508}"/>
-    <hyperlink ref="A27" r:id="rId27" display="http://www.worldsurfleague.com/athletes/700/jesse-mendes" xr:uid="{468C63BF-B21F-4854-B0A6-E7425EF25496}"/>
-    <hyperlink ref="A28" r:id="rId28" display="http://www.worldsurfleague.com/athletes/2760/deivid-silva" xr:uid="{1C3A2C40-6856-4311-9489-99F10D25358E}"/>
-    <hyperlink ref="A29" r:id="rId29" display="http://www.worldsurfleague.com/athletes/314/ricardo-christie" xr:uid="{6E8CBA16-F1BD-4110-89A9-37E77CE121FE}"/>
-    <hyperlink ref="A30" r:id="rId30" display="http://www.worldsurfleague.com/athletes/2656/leonardo-fioravanti" xr:uid="{E8CC9442-00D3-4B4F-9EA0-AFB764984B7F}"/>
-    <hyperlink ref="A31" r:id="rId31" display="http://www.worldsurfleague.com/athletes/466/jadson-andre" xr:uid="{DCAEAD23-FC05-4E42-A6E2-26FC00212FA2}"/>
-    <hyperlink ref="A32" r:id="rId32" display="http://www.worldsurfleague.com/athletes/2824/soli-bailey" xr:uid="{5E8169BE-67CB-4C4B-A398-53704BA3B0F1}"/>
-    <hyperlink ref="A33" r:id="rId33" display="http://www.worldsurfleague.com/athletes/2112/jack-freestone" xr:uid="{854F204E-AD87-4D7A-B029-D0F8EC044F21}"/>
-    <hyperlink ref="A34" r:id="rId34" display="http://www.worldsurfleague.com/athletes/553/kelly-slater" xr:uid="{55475A73-0DB5-4913-8704-31CF996CEB64}"/>
-  </hyperlinks>
+  <autoFilter ref="A1:D38" xr:uid="{699AD27B-32D7-4E18-A927-E4BB453C8670}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>